<commit_message>
used simple pt_pathfinder to decrease file size. continued preperation for exc 3.
</commit_message>
<xml_diff>
--- a/input/transport_stats/strecke_wegzwecke_mid17_t9.xlsx
+++ b/input/transport_stats/strecke_wegzwecke_mid17_t9.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Wegzweck</t>
   </si>
@@ -31,31 +31,52 @@
     <t xml:space="preserve">Quelle</t>
   </si>
   <si>
+    <t xml:space="preserve">Work </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MiD 2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arbeit</t>
   </si>
   <si>
-    <t xml:space="preserve">MiD 2017</t>
+    <t xml:space="preserve">Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabelle 9</t>
   </si>
   <si>
     <t xml:space="preserve">dienstlich</t>
   </si>
   <si>
-    <t xml:space="preserve">Tabelle 9</t>
+    <t xml:space="preserve">Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">durchschnittliche Wegelämgen in Metropolen</t>
   </si>
   <si>
     <t xml:space="preserve">Ausbildung</t>
   </si>
   <si>
-    <t xml:space="preserve">durchschnittliche Wegelämgen in Metropolen</t>
+    <t xml:space="preserve">Shopping </t>
   </si>
   <si>
     <t xml:space="preserve">Einkauf</t>
   </si>
   <si>
+    <t xml:space="preserve">Errands</t>
+  </si>
+  <si>
     <t xml:space="preserve">Erledigung</t>
   </si>
   <si>
+    <t xml:space="preserve">Leisure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freizeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accompaniment </t>
   </si>
   <si>
     <t xml:space="preserve">Begleitung</t>
@@ -133,13 +154,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -162,10 +187,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -183,9 +208,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -194,60 +222,81 @@
       <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>12</v>
+      <c r="A8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
corrected mistake in pois that craft keys are lost
</commit_message>
<xml_diff>
--- a/input/transport_stats/strecke_wegzwecke_mid17_t9.xlsx
+++ b/input/transport_stats/strecke_wegzwecke_mid17_t9.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Quelle</t>
   </si>
   <si>
-    <t xml:space="preserve">Work </t>
+    <t xml:space="preserve">Work</t>
   </si>
   <si>
     <t xml:space="preserve">MiD 2017</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Ausbildung</t>
   </si>
   <si>
-    <t xml:space="preserve">Shopping </t>
+    <t xml:space="preserve">Shopping</t>
   </si>
   <si>
     <t xml:space="preserve">Einkauf</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Freizeit</t>
   </si>
   <si>
-    <t xml:space="preserve">Accompaniment </t>
+    <t xml:space="preserve">Accompaniment</t>
   </si>
   <si>
     <t xml:space="preserve">Begleitung</t>
@@ -187,10 +187,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>

</xml_diff>